<commit_message>
Fix #4005 Model ISA-TAB-MODEL.xlsx import error
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/ISA-TAB-MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/ISA-TAB-MODEL.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="3040" windowWidth="28420" windowHeight="15500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3645" yWindow="3045" windowWidth="28425" windowHeight="15495" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="410">
   <si>
     <t>name</t>
   </si>
@@ -904,6 +904,354 @@
   </si>
   <si>
     <t>ISATAB</t>
+  </si>
+  <si>
+    <t>inv_Identifier</t>
+  </si>
+  <si>
+    <t>inv_Title</t>
+  </si>
+  <si>
+    <t>inv_Description</t>
+  </si>
+  <si>
+    <t>inv_Submission_Date</t>
+  </si>
+  <si>
+    <t>inv_Public_Release_Date</t>
+  </si>
+  <si>
+    <t>Term_src_name</t>
+  </si>
+  <si>
+    <t>Term_src_File</t>
+  </si>
+  <si>
+    <t>Term_src_Version</t>
+  </si>
+  <si>
+    <t>Term_src_Description</t>
+  </si>
+  <si>
+    <t>inv_PubMed_ID</t>
+  </si>
+  <si>
+    <t>inv_pub_DOI</t>
+  </si>
+  <si>
+    <t>inv_pub_Author_List</t>
+  </si>
+  <si>
+    <t>inv_pub_Title</t>
+  </si>
+  <si>
+    <t>inv_pub_Status</t>
+  </si>
+  <si>
+    <t>inv_pub_Status_Term_acc_num</t>
+  </si>
+  <si>
+    <t>inv_pub_Status_Term_src_REF</t>
+  </si>
+  <si>
+    <t>inv_Person_Last_Name</t>
+  </si>
+  <si>
+    <t>inv_Person_First_Name</t>
+  </si>
+  <si>
+    <t>inv_Person_Mid_Initials</t>
+  </si>
+  <si>
+    <t>inv_Person_Email</t>
+  </si>
+  <si>
+    <t>inv_Person_Phone</t>
+  </si>
+  <si>
+    <t>inv_Person_Fax</t>
+  </si>
+  <si>
+    <t>inv_Person_Address</t>
+  </si>
+  <si>
+    <t>inv_Person_Affiliation</t>
+  </si>
+  <si>
+    <t>inv_Person_Roles_</t>
+  </si>
+  <si>
+    <t>inv_Person_Roles_Term_acc_num</t>
+  </si>
+  <si>
+    <t>inv_Person_Roles_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Identifier</t>
+  </si>
+  <si>
+    <t>st_Title</t>
+  </si>
+  <si>
+    <t>st_Description</t>
+  </si>
+  <si>
+    <t>st_Submission_Date</t>
+  </si>
+  <si>
+    <t>st_Public_Release_Date</t>
+  </si>
+  <si>
+    <t>st_File_Name</t>
+  </si>
+  <si>
+    <t>st_Design_tp</t>
+  </si>
+  <si>
+    <t>st_Design_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_Design_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_PubMed_ID</t>
+  </si>
+  <si>
+    <t>st_pub_DOI</t>
+  </si>
+  <si>
+    <t>st_pub_Author_List</t>
+  </si>
+  <si>
+    <t>st_pub_Title</t>
+  </si>
+  <si>
+    <t>st_pub_Status</t>
+  </si>
+  <si>
+    <t>st_pub_Status_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_pub_Status_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Factor_Name</t>
+  </si>
+  <si>
+    <t>st_Factor_tp</t>
+  </si>
+  <si>
+    <t>st_Factor_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_Factor_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Assay_meas_tp</t>
+  </si>
+  <si>
+    <t>st_Assay_meas_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_Assay_meas_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Assay_tech_tp</t>
+  </si>
+  <si>
+    <t>st_Assay_tech_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_Assay_tech_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Assay_tech_Platform</t>
+  </si>
+  <si>
+    <t>st_Assay_File_Name</t>
+  </si>
+  <si>
+    <t>st_prot_Name</t>
+  </si>
+  <si>
+    <t>st_prot_tp</t>
+  </si>
+  <si>
+    <t>st_prot_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_prot_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_prot_Description</t>
+  </si>
+  <si>
+    <t>st_prot_URI</t>
+  </si>
+  <si>
+    <t>st_prot_Version</t>
+  </si>
+  <si>
+    <t>st_prot_params_Name</t>
+  </si>
+  <si>
+    <t>st_prot_params_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_prot_params_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_prot_comps_Name</t>
+  </si>
+  <si>
+    <t>st_prot_comps_tp</t>
+  </si>
+  <si>
+    <t>st_prot_comps_tp_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_prot_comps_tp_Term_src_REF</t>
+  </si>
+  <si>
+    <t>st_Person_Last_Name</t>
+  </si>
+  <si>
+    <t>st_Person_First_Name</t>
+  </si>
+  <si>
+    <t>st_Person_Mid_Initials</t>
+  </si>
+  <si>
+    <t>st_Person_Email</t>
+  </si>
+  <si>
+    <t>st_Person_Phone</t>
+  </si>
+  <si>
+    <t>st_Person_Fax</t>
+  </si>
+  <si>
+    <t>st_Person_Address</t>
+  </si>
+  <si>
+    <t>st_Person_Affiliation</t>
+  </si>
+  <si>
+    <t>st_Person_Roles_</t>
+  </si>
+  <si>
+    <t>st_Person_Roles_Term_acc_num</t>
+  </si>
+  <si>
+    <t>st_Person_Roles_Term_src_REF</t>
+  </si>
+  <si>
+    <t>Source_Name</t>
+  </si>
+  <si>
+    <t>Sample_Name</t>
+  </si>
+  <si>
+    <t>Material_tp</t>
+  </si>
+  <si>
+    <t>Protocol_REF</t>
+  </si>
+  <si>
+    <t>Term_acc_num</t>
+  </si>
+  <si>
+    <t>Term_src_REF</t>
+  </si>
+  <si>
+    <t>Factor_Value</t>
+  </si>
+  <si>
+    <t>Sample_Name_</t>
+  </si>
+  <si>
+    <t>Extract_Name_</t>
+  </si>
+  <si>
+    <t>Labeled_Extract_Name_</t>
+  </si>
+  <si>
+    <t>Image_File</t>
+  </si>
+  <si>
+    <t>Raw_Data_File</t>
+  </si>
+  <si>
+    <t>Data_Transformation_Name</t>
+  </si>
+  <si>
+    <t>Normalization_Name</t>
+  </si>
+  <si>
+    <t>Derived_Data_File</t>
+  </si>
+  <si>
+    <t>Hybridization_Assay_Name</t>
+  </si>
+  <si>
+    <t>Scan_Name</t>
+  </si>
+  <si>
+    <t>Array_Data_File</t>
+  </si>
+  <si>
+    <t>Derived_Array_Data_File</t>
+  </si>
+  <si>
+    <t>Array_Data_Matrix_File</t>
+  </si>
+  <si>
+    <t>Derived_Array_Data_Matrix_File</t>
+  </si>
+  <si>
+    <t>Array_Design_File</t>
+  </si>
+  <si>
+    <t>Array_Design_REF</t>
+  </si>
+  <si>
+    <t>Gel_Electrophoresis_Assay_Name</t>
+  </si>
+  <si>
+    <t>First_Dimension_</t>
+  </si>
+  <si>
+    <t>Second_Dimension</t>
+  </si>
+  <si>
+    <t>Spot_Picking_File</t>
+  </si>
+  <si>
+    <t>MS_Assay_Name</t>
+  </si>
+  <si>
+    <t>Raw_Spectral_Data_File</t>
+  </si>
+  <si>
+    <t>Derived_Spectral_Data_File</t>
+  </si>
+  <si>
+    <t>Peptide_Assignment_File</t>
+  </si>
+  <si>
+    <t>Protein_Assignment_File</t>
+  </si>
+  <si>
+    <t>Post_trans_mode_ass_file</t>
+  </si>
+  <si>
+    <t>NMR_Assay_Name</t>
+  </si>
+  <si>
+    <t>Free_Induct_Decay_Data_File_</t>
+  </si>
+  <si>
+    <t>Acq_Parameter_Data_File_</t>
   </si>
 </sst>
 </file>
@@ -1567,6 +1915,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1898,13 +2251,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1918,7 +2271,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1929,7 +2282,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>202</v>
       </c>
@@ -1940,7 +2293,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>203</v>
       </c>
@@ -1951,7 +2304,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -1962,7 +2315,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>212</v>
       </c>
@@ -1976,7 +2329,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>218</v>
       </c>
@@ -1990,7 +2343,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -2004,7 +2357,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>226</v>
       </c>
@@ -2031,87 +2384,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P131"/>
+  <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H127" sqref="H127"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1" t="b">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="b">
+      <c r="G2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -2120,18 +2478,21 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -2144,18 +2505,21 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -2168,18 +2532,21 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -2192,18 +2559,21 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2216,1442 +2586,1818 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B9" t="s">
         <v>47</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>39</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" t="s">
         <v>61</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" t="s">
         <v>74</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>39</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>306</v>
+      </c>
+      <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>39</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" t="s">
         <v>68</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>310</v>
+      </c>
+      <c r="B18" t="s">
         <v>75</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>311</v>
+      </c>
+      <c r="B19" t="s">
         <v>77</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>312</v>
+      </c>
+      <c r="B20" t="s">
         <v>79</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>39</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>313</v>
+      </c>
+      <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>39</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>314</v>
+      </c>
+      <c r="B22" t="s">
         <v>83</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>315</v>
+      </c>
+      <c r="B23" t="s">
         <v>85</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>39</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>316</v>
+      </c>
+      <c r="B24" t="s">
         <v>87</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>39</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="16" customHeight="1">
+    <row r="25" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>317</v>
+      </c>
+      <c r="B25" t="s">
         <v>89</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>39</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="16" customHeight="1">
+    <row r="26" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" t="s">
         <v>91</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="16" customHeight="1">
+    <row r="27" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>319</v>
+      </c>
+      <c r="B27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="16" customHeight="1">
+    <row r="28" spans="1:17" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>320</v>
+      </c>
+      <c r="B28" t="s">
         <v>93</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>39</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>294</v>
+      </c>
+      <c r="B29" t="s">
         <v>51</v>
       </c>
-      <c r="B29" t="s">
-        <v>202</v>
-      </c>
       <c r="C29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D29" t="s">
         <v>42</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>39</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>321</v>
+      </c>
+      <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="B30" t="s">
-        <v>202</v>
-      </c>
-      <c r="E30" t="b">
+      <c r="C30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F30" t="b">
         <v>1</v>
       </c>
-      <c r="F30" s="1" t="b">
+      <c r="G30" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>322</v>
+      </c>
+      <c r="B31" t="s">
         <v>97</v>
       </c>
-      <c r="B31" t="s">
-        <v>202</v>
-      </c>
-      <c r="P31" t="s">
+      <c r="C31" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B32" t="s">
         <v>99</v>
       </c>
-      <c r="B32" t="s">
-        <v>202</v>
-      </c>
-      <c r="P32" t="s">
+      <c r="C32" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>324</v>
+      </c>
+      <c r="B33" t="s">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
-        <v>202</v>
-      </c>
-      <c r="P33" t="s">
+      <c r="C33" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>325</v>
+      </c>
+      <c r="B34" t="s">
         <v>103</v>
       </c>
-      <c r="B34" t="s">
-        <v>202</v>
-      </c>
-      <c r="P34" t="s">
+      <c r="C34" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q34" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>326</v>
+      </c>
+      <c r="B35" t="s">
         <v>105</v>
       </c>
-      <c r="B35" t="s">
-        <v>202</v>
-      </c>
-      <c r="P35" t="s">
+      <c r="C35" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>327</v>
+      </c>
+      <c r="B36" t="s">
         <v>107</v>
       </c>
-      <c r="B36" t="s">
-        <v>202</v>
-      </c>
-      <c r="P36" t="s">
+      <c r="C36" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q36" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>328</v>
+      </c>
+      <c r="B37" t="s">
         <v>108</v>
       </c>
-      <c r="B37" t="s">
-        <v>202</v>
-      </c>
-      <c r="P37" t="s">
+      <c r="C37" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>329</v>
+      </c>
+      <c r="B38" t="s">
         <v>109</v>
       </c>
-      <c r="B38" t="s">
-        <v>202</v>
-      </c>
-      <c r="P38" t="s">
+      <c r="C38" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q38" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>330</v>
+      </c>
+      <c r="B39" t="s">
         <v>112</v>
       </c>
-      <c r="B39" t="s">
-        <v>202</v>
-      </c>
-      <c r="P39" t="s">
+      <c r="C39" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>331</v>
+      </c>
+      <c r="B40" t="s">
         <v>114</v>
       </c>
-      <c r="B40" t="s">
-        <v>202</v>
-      </c>
-      <c r="P40" t="s">
+      <c r="C40" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q40" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>332</v>
+      </c>
+      <c r="B41" t="s">
         <v>116</v>
       </c>
-      <c r="B41" t="s">
-        <v>202</v>
-      </c>
-      <c r="P41" t="s">
+      <c r="C41" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q41" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>333</v>
+      </c>
+      <c r="B42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" t="s">
-        <v>202</v>
-      </c>
-      <c r="P42" t="s">
+      <c r="C42" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q42" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>334</v>
+      </c>
+      <c r="B43" t="s">
         <v>120</v>
       </c>
-      <c r="B43" t="s">
-        <v>202</v>
-      </c>
-      <c r="P43" t="s">
+      <c r="C43" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q43" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>335</v>
+      </c>
+      <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="B44" t="s">
-        <v>202</v>
-      </c>
-      <c r="P44" t="s">
+      <c r="C44" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q44" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>336</v>
+      </c>
+      <c r="B45" t="s">
         <v>122</v>
       </c>
-      <c r="B45" t="s">
-        <v>202</v>
-      </c>
-      <c r="P45" t="s">
+      <c r="C45" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q45" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>337</v>
+      </c>
+      <c r="B46" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
-        <v>202</v>
-      </c>
-      <c r="P46" t="s">
+      <c r="C46" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q46" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>338</v>
+      </c>
+      <c r="B47" t="s">
         <v>125</v>
       </c>
-      <c r="B47" t="s">
-        <v>202</v>
-      </c>
-      <c r="P47" t="s">
+      <c r="C47" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q47" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>339</v>
+      </c>
+      <c r="B48" t="s">
         <v>126</v>
       </c>
-      <c r="B48" t="s">
-        <v>202</v>
-      </c>
-      <c r="P48" t="s">
+      <c r="C48" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q48" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>340</v>
+      </c>
+      <c r="B49" t="s">
         <v>127</v>
       </c>
-      <c r="B49" t="s">
-        <v>202</v>
-      </c>
-      <c r="P49" t="s">
+      <c r="C49" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q49" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>341</v>
+      </c>
+      <c r="B50" t="s">
         <v>131</v>
       </c>
-      <c r="B50" t="s">
-        <v>202</v>
-      </c>
-      <c r="P50" t="s">
+      <c r="C50" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q50" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>342</v>
+      </c>
+      <c r="B51" t="s">
         <v>132</v>
       </c>
-      <c r="B51" t="s">
-        <v>202</v>
-      </c>
-      <c r="P51" t="s">
+      <c r="C51" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>343</v>
+      </c>
+      <c r="B52" t="s">
         <v>133</v>
       </c>
-      <c r="B52" t="s">
-        <v>202</v>
-      </c>
-      <c r="P52" t="s">
+      <c r="C52" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q52" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>344</v>
+      </c>
+      <c r="B53" t="s">
         <v>134</v>
       </c>
-      <c r="B53" t="s">
-        <v>202</v>
-      </c>
-      <c r="P53" t="s">
+      <c r="C53" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q53" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>345</v>
+      </c>
+      <c r="B54" t="s">
         <v>135</v>
       </c>
-      <c r="B54" t="s">
-        <v>202</v>
-      </c>
-      <c r="P54" t="s">
+      <c r="C54" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q54" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>346</v>
+      </c>
+      <c r="B55" t="s">
         <v>136</v>
       </c>
-      <c r="B55" t="s">
-        <v>202</v>
-      </c>
-      <c r="P55" t="s">
+      <c r="C55" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q55" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>347</v>
+      </c>
+      <c r="B56" t="s">
         <v>137</v>
       </c>
-      <c r="B56" t="s">
-        <v>202</v>
-      </c>
-      <c r="P56" t="s">
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q56" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>348</v>
+      </c>
+      <c r="B57" t="s">
         <v>138</v>
       </c>
-      <c r="B57" t="s">
-        <v>202</v>
-      </c>
-      <c r="P57" t="s">
+      <c r="C57" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q57" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>349</v>
+      </c>
+      <c r="B58" t="s">
         <v>152</v>
       </c>
-      <c r="B58" t="s">
-        <v>202</v>
-      </c>
-      <c r="P58" t="s">
+      <c r="C58" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q58" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>350</v>
+      </c>
+      <c r="B59" t="s">
         <v>153</v>
       </c>
-      <c r="B59" t="s">
-        <v>202</v>
-      </c>
-      <c r="P59" t="s">
+      <c r="C59" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q59" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>351</v>
+      </c>
+      <c r="B60" t="s">
         <v>156</v>
       </c>
-      <c r="B60" t="s">
-        <v>202</v>
-      </c>
-      <c r="P60" t="s">
+      <c r="C60" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q60" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>352</v>
+      </c>
+      <c r="B61" t="s">
         <v>157</v>
       </c>
-      <c r="B61" t="s">
-        <v>202</v>
-      </c>
-      <c r="P61" t="s">
+      <c r="C61" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q61" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>353</v>
+      </c>
+      <c r="B62" t="s">
         <v>144</v>
       </c>
-      <c r="B62" t="s">
-        <v>202</v>
-      </c>
-      <c r="P62" t="s">
+      <c r="C62" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q62" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>354</v>
+      </c>
+      <c r="B63" t="s">
         <v>145</v>
       </c>
-      <c r="B63" t="s">
-        <v>202</v>
-      </c>
-      <c r="P63" t="s">
+      <c r="C63" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q63" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>355</v>
+      </c>
+      <c r="B64" t="s">
         <v>146</v>
       </c>
-      <c r="B64" t="s">
-        <v>202</v>
-      </c>
-      <c r="P64" t="s">
+      <c r="C64" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q64" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>356</v>
+      </c>
+      <c r="B65" t="s">
         <v>161</v>
       </c>
-      <c r="B65" t="s">
-        <v>202</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="C65" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q65" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>357</v>
+      </c>
+      <c r="B66" t="s">
         <v>147</v>
       </c>
-      <c r="B66" t="s">
-        <v>202</v>
-      </c>
-      <c r="P66" t="s">
+      <c r="C66" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q66" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>358</v>
+      </c>
+      <c r="B67" t="s">
         <v>148</v>
       </c>
-      <c r="B67" t="s">
-        <v>202</v>
-      </c>
-      <c r="P67" t="s">
+      <c r="C67" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q67" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>359</v>
+      </c>
+      <c r="B68" t="s">
         <v>149</v>
       </c>
-      <c r="B68" t="s">
-        <v>202</v>
-      </c>
-      <c r="P68" t="s">
+      <c r="C68" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q68" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>360</v>
+      </c>
+      <c r="B69" t="s">
         <v>150</v>
       </c>
-      <c r="B69" t="s">
-        <v>202</v>
-      </c>
-      <c r="P69" t="s">
+      <c r="C69" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q69" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>361</v>
+      </c>
+      <c r="B70" t="s">
         <v>166</v>
       </c>
-      <c r="B70" t="s">
-        <v>202</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="C70" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q70" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>362</v>
+      </c>
+      <c r="B71" t="s">
         <v>151</v>
       </c>
-      <c r="B71" t="s">
-        <v>202</v>
-      </c>
-      <c r="P71" t="s">
+      <c r="C71" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q71" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>363</v>
+      </c>
+      <c r="B72" t="s">
         <v>168</v>
       </c>
-      <c r="B72" t="s">
-        <v>202</v>
-      </c>
-      <c r="P72" t="s">
+      <c r="C72" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q72" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>364</v>
+      </c>
+      <c r="B73" t="s">
         <v>170</v>
       </c>
-      <c r="B73" t="s">
-        <v>202</v>
-      </c>
-      <c r="P73" t="s">
+      <c r="C73" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q73" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>365</v>
+      </c>
+      <c r="B74" t="s">
         <v>172</v>
       </c>
-      <c r="B74" t="s">
-        <v>202</v>
-      </c>
-      <c r="P74" t="s">
+      <c r="C74" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q74" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>366</v>
+      </c>
+      <c r="B75" t="s">
         <v>174</v>
       </c>
-      <c r="B75" t="s">
-        <v>202</v>
-      </c>
-      <c r="P75" t="s">
+      <c r="C75" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q75" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>367</v>
+      </c>
+      <c r="B76" t="s">
         <v>176</v>
       </c>
-      <c r="B76" t="s">
-        <v>202</v>
-      </c>
-      <c r="P76" t="s">
+      <c r="C76" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q76" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>368</v>
+      </c>
+      <c r="B77" t="s">
         <v>178</v>
       </c>
-      <c r="B77" t="s">
-        <v>202</v>
-      </c>
-      <c r="P77" t="s">
+      <c r="C77" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q77" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>369</v>
+      </c>
+      <c r="B78" t="s">
         <v>180</v>
       </c>
-      <c r="B78" t="s">
-        <v>202</v>
-      </c>
-      <c r="P78" t="s">
+      <c r="C78" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q78" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>370</v>
+      </c>
+      <c r="B79" t="s">
         <v>182</v>
       </c>
-      <c r="B79" t="s">
-        <v>202</v>
-      </c>
-      <c r="P79" t="s">
+      <c r="C79" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q79" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>371</v>
+      </c>
+      <c r="B80" t="s">
         <v>184</v>
       </c>
-      <c r="B80" t="s">
-        <v>202</v>
-      </c>
-      <c r="P80" t="s">
+      <c r="C80" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q80" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>372</v>
+      </c>
+      <c r="B81" t="s">
         <v>185</v>
       </c>
-      <c r="B81" t="s">
-        <v>202</v>
-      </c>
-      <c r="P81" t="s">
+      <c r="C81" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q81" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>373</v>
+      </c>
+      <c r="B82" t="s">
         <v>186</v>
       </c>
-      <c r="B82" t="s">
-        <v>202</v>
-      </c>
-      <c r="P82" t="s">
+      <c r="C82" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q82" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>203</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>41</v>
       </c>
-      <c r="D83" t="s">
-        <v>202</v>
-      </c>
-      <c r="P83" t="s">
+      <c r="E83" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q83" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>374</v>
+      </c>
+      <c r="B84" t="s">
         <v>26</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>203</v>
       </c>
-      <c r="P84" t="s">
+      <c r="Q84" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>375</v>
+      </c>
+      <c r="B85" t="s">
         <v>19</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>203</v>
       </c>
-      <c r="E85" t="b">
+      <c r="F85" t="b">
         <v>1</v>
       </c>
-      <c r="F85" s="1" t="b">
+      <c r="G85" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P85" t="s">
+      <c r="Q85" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>376</v>
+      </c>
+      <c r="B86" t="s">
         <v>20</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>203</v>
       </c>
-      <c r="P86" t="s">
+      <c r="Q86" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>196</v>
       </c>
       <c r="B87" t="s">
+        <v>196</v>
+      </c>
+      <c r="C87" t="s">
         <v>203</v>
       </c>
-      <c r="P87" t="s">
+      <c r="Q87" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>197</v>
       </c>
       <c r="B88" t="s">
+        <v>197</v>
+      </c>
+      <c r="C88" t="s">
         <v>203</v>
       </c>
-      <c r="P88" t="s">
+      <c r="Q88" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>377</v>
+      </c>
+      <c r="B89" t="s">
         <v>23</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>203</v>
       </c>
-      <c r="P89" t="s">
+      <c r="Q89" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>378</v>
+      </c>
+      <c r="B90" t="s">
         <v>22</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>203</v>
       </c>
-      <c r="P90" t="s">
+      <c r="Q90" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>379</v>
+      </c>
+      <c r="B91" t="s">
         <v>21</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>203</v>
       </c>
-      <c r="P91" t="s">
+      <c r="Q91" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>380</v>
+      </c>
+      <c r="B92" t="s">
         <v>200</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>203</v>
       </c>
-      <c r="P92" t="s">
+      <c r="Q92" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>201</v>
       </c>
       <c r="B93" t="s">
+        <v>201</v>
+      </c>
+      <c r="C93" t="s">
         <v>203</v>
       </c>
-      <c r="P93" t="s">
+      <c r="Q93" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>381</v>
+      </c>
+      <c r="B94" t="s">
         <v>206</v>
       </c>
-      <c r="B94" t="s">
+      <c r="C94" t="s">
         <v>204</v>
       </c>
-      <c r="C94" t="s">
+      <c r="D94" t="s">
         <v>41</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>203</v>
       </c>
-      <c r="P94" t="s">
+      <c r="Q94" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>382</v>
+      </c>
+      <c r="B95" t="s">
         <v>207</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" t="s">
         <v>204</v>
       </c>
-      <c r="E95" t="b">
+      <c r="F95" t="b">
         <v>1</v>
       </c>
-      <c r="F95" s="1" t="b">
+      <c r="G95" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P95" t="s">
+      <c r="Q95" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>383</v>
+      </c>
+      <c r="B96" t="s">
         <v>208</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" t="s">
         <v>204</v>
       </c>
-      <c r="P96" t="s">
+      <c r="Q96" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>384</v>
+      </c>
+      <c r="B97" t="s">
         <v>209</v>
       </c>
-      <c r="B97" t="s">
+      <c r="C97" t="s">
         <v>204</v>
       </c>
-      <c r="P97" t="s">
+      <c r="Q97" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>385</v>
+      </c>
+      <c r="B98" t="s">
         <v>210</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>204</v>
       </c>
-      <c r="P98" t="s">
+      <c r="Q98" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>386</v>
+      </c>
+      <c r="B99" t="s">
         <v>32</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" t="s">
         <v>204</v>
       </c>
-      <c r="P99" t="s">
+      <c r="Q99" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>387</v>
+      </c>
+      <c r="B100" t="s">
         <v>34</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" t="s">
         <v>204</v>
       </c>
-      <c r="P100" t="s">
+      <c r="Q100" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>388</v>
+      </c>
+      <c r="B101" t="s">
         <v>211</v>
       </c>
-      <c r="B101" t="s">
+      <c r="C101" t="s">
         <v>204</v>
       </c>
-      <c r="P101" t="s">
+      <c r="Q101" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>376</v>
+      </c>
+      <c r="B102" t="s">
         <v>20</v>
       </c>
-      <c r="B102" t="s">
+      <c r="C102" t="s">
         <v>204</v>
       </c>
-      <c r="P102" t="s">
+      <c r="Q102" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>196</v>
       </c>
       <c r="B103" t="s">
+        <v>196</v>
+      </c>
+      <c r="C103" t="s">
         <v>204</v>
       </c>
-      <c r="P103" t="s">
+      <c r="Q103" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>27</v>
       </c>
       <c r="B104" t="s">
+        <v>27</v>
+      </c>
+      <c r="C104" t="s">
         <v>204</v>
       </c>
-      <c r="P104" t="s">
+      <c r="Q104" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>377</v>
+      </c>
+      <c r="B105" t="s">
         <v>23</v>
       </c>
-      <c r="B105" t="s">
+      <c r="C105" t="s">
         <v>204</v>
       </c>
-      <c r="P105" t="s">
+      <c r="Q105" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
+        <v>378</v>
+      </c>
+      <c r="B106" t="s">
         <v>22</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>204</v>
       </c>
-      <c r="P106" t="s">
+      <c r="Q106" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>379</v>
+      </c>
+      <c r="B107" t="s">
         <v>21</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>204</v>
       </c>
-      <c r="P107" t="s">
+      <c r="Q107" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>201</v>
       </c>
       <c r="B108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
         <v>204</v>
       </c>
-      <c r="P108" t="s">
+      <c r="Q108" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>389</v>
+      </c>
+      <c r="B109" t="s">
         <v>28</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" t="s">
         <v>212</v>
       </c>
-      <c r="E109" t="b">
+      <c r="F109" t="b">
         <v>1</v>
       </c>
-      <c r="F109" s="1" t="b">
+      <c r="G109" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P109" t="s">
+      <c r="Q109" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>390</v>
+      </c>
+      <c r="B110" t="s">
         <v>30</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>212</v>
       </c>
-      <c r="P110" t="s">
+      <c r="Q110" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>391</v>
+      </c>
+      <c r="B111" t="s">
         <v>31</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>212</v>
       </c>
-      <c r="P111" t="s">
+      <c r="Q111" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>392</v>
+      </c>
+      <c r="B112" t="s">
         <v>33</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>212</v>
       </c>
-      <c r="P112" t="s">
+      <c r="Q112" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>393</v>
+      </c>
+      <c r="B113" t="s">
         <v>215</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
         <v>212</v>
       </c>
-      <c r="P113" t="s">
+      <c r="Q113" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>394</v>
+      </c>
+      <c r="B114" t="s">
         <v>216</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>212</v>
       </c>
-      <c r="P114" t="s">
+      <c r="Q114" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>395</v>
+      </c>
+      <c r="B115" t="s">
         <v>217</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>212</v>
       </c>
-      <c r="P115" t="s">
+      <c r="Q115" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
+        <v>396</v>
+      </c>
+      <c r="B116" t="s">
         <v>29</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>212</v>
       </c>
-      <c r="P116" t="s">
+      <c r="Q116" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
+        <v>397</v>
+      </c>
+      <c r="B117" t="s">
         <v>220</v>
       </c>
-      <c r="B117" t="s">
+      <c r="C117" t="s">
         <v>218</v>
       </c>
-      <c r="E117" t="b">
+      <c r="F117" t="b">
         <v>1</v>
       </c>
-      <c r="F117" s="1" t="b">
+      <c r="G117" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P117" t="s">
+      <c r="Q117" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
+        <v>398</v>
+      </c>
+      <c r="B118" t="s">
         <v>221</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>218</v>
       </c>
-      <c r="P118" t="s">
+      <c r="Q118" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>399</v>
+      </c>
+      <c r="B119" t="s">
         <v>222</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>218</v>
       </c>
-      <c r="P119" t="s">
+      <c r="Q119" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>390</v>
+      </c>
+      <c r="B120" t="s">
         <v>30</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>218</v>
       </c>
-      <c r="P120" t="s">
+      <c r="Q120" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>400</v>
+      </c>
+      <c r="B121" t="s">
         <v>223</v>
       </c>
-      <c r="B121" t="s">
+      <c r="C121" t="s">
         <v>218</v>
       </c>
-      <c r="P121" t="s">
+      <c r="Q121" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>401</v>
+      </c>
+      <c r="B122" t="s">
         <v>24</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>224</v>
       </c>
-      <c r="E122" t="b">
+      <c r="F122" t="b">
         <v>1</v>
       </c>
-      <c r="F122" s="1" t="b">
+      <c r="G122" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P122" t="s">
+      <c r="Q122" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>402</v>
+      </c>
+      <c r="B123" t="s">
         <v>25</v>
       </c>
-      <c r="B123" t="s">
+      <c r="C123" t="s">
         <v>224</v>
       </c>
-      <c r="P123" t="s">
+      <c r="Q123" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
+        <v>403</v>
+      </c>
+      <c r="B124" t="s">
         <v>38</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>224</v>
       </c>
-      <c r="P124" t="s">
+      <c r="Q124" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
+        <v>404</v>
+      </c>
+      <c r="B125" t="s">
         <v>36</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>224</v>
       </c>
-      <c r="P125" t="s">
+      <c r="Q125" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>405</v>
+      </c>
+      <c r="B126" t="s">
         <v>35</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>224</v>
       </c>
-      <c r="P126" t="s">
+      <c r="Q126" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>406</v>
+      </c>
+      <c r="B127" t="s">
         <v>37</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>224</v>
       </c>
-      <c r="P127" t="s">
+      <c r="Q127" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>407</v>
+      </c>
+      <c r="B128" t="s">
         <v>228</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
         <v>226</v>
       </c>
-      <c r="E128" t="b">
+      <c r="F128" t="b">
         <v>1</v>
       </c>
-      <c r="F128" s="1" t="b">
+      <c r="G128" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="P128" t="s">
+      <c r="Q128" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>408</v>
+      </c>
+      <c r="B129" t="s">
         <v>229</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>226</v>
       </c>
-      <c r="P129" t="s">
+      <c r="Q129" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
+        <v>409</v>
+      </c>
+      <c r="B130" t="s">
         <v>230</v>
       </c>
-      <c r="B130" t="s">
+      <c r="C130" t="s">
         <v>226</v>
       </c>
-      <c r="P130" t="s">
+      <c r="Q130" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>403</v>
+      </c>
+      <c r="B131" t="s">
         <v>38</v>
       </c>
-      <c r="B131" t="s">
+      <c r="C131" t="s">
         <v>226</v>
       </c>
-      <c r="P131" t="s">
+      <c r="Q131" t="s">
         <v>262</v>
       </c>
     </row>
@@ -3670,17 +4416,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="84.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3694,7 +4440,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -3724,16 +4470,16 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="69.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="69.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>266</v>
       </c>
@@ -3753,7 +4499,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>275</v>
       </c>
@@ -3773,7 +4519,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>276</v>
       </c>
@@ -3793,7 +4539,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>278</v>
       </c>
@@ -3813,7 +4559,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>281</v>
       </c>
@@ -3833,7 +4579,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>283</v>
       </c>
@@ -3853,7 +4599,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>286</v>
       </c>
@@ -3873,7 +4619,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>287</v>
       </c>
@@ -3893,7 +4639,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>291</v>
       </c>

</xml_diff>

<commit_message>
Resolve missing idAttribute errors
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/ISA-TAB-MODEL.xlsx
+++ b/molgenis-model-registry/src/test/resources/ISA-TAB-MODEL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="3045" windowWidth="28425" windowHeight="15495" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3645" yWindow="3045" windowWidth="28425" windowHeight="15495" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="entities" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="packages" sheetId="3" r:id="rId3"/>
     <sheet name="tags" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="418">
   <si>
     <t>name</t>
   </si>
@@ -1252,6 +1252,30 @@
   </si>
   <si>
     <t>Acq_Parameter_Data_File_</t>
+  </si>
+  <si>
+    <t>ISATAB_Investigation</t>
+  </si>
+  <si>
+    <t>ISATAB_Study_Section</t>
+  </si>
+  <si>
+    <t>ISATAB_Study_Node</t>
+  </si>
+  <si>
+    <t>ISATAB_Assay_Node</t>
+  </si>
+  <si>
+    <t>ISATAB_Assay_Microarray</t>
+  </si>
+  <si>
+    <t>ISATAB_Assay_Electrophoresis</t>
+  </si>
+  <si>
+    <t>ISATAB_Assay_MS</t>
+  </si>
+  <si>
+    <t>ISATAB_Assay_NMR</t>
   </si>
 </sst>
 </file>
@@ -2247,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2326,7 +2350,7 @@
         <v>214</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,7 +2364,7 @@
         <v>219</v>
       </c>
       <c r="D7" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2354,7 +2378,7 @@
         <v>225</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2368,7 +2392,7 @@
         <v>227</v>
       </c>
       <c r="D9" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
     </row>
   </sheetData>
@@ -2386,14 +2410,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A131"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
@@ -2460,7 +2486,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -2491,7 +2517,7 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2518,7 +2544,7 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2545,7 +2571,7 @@
         <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -2572,7 +2598,7 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -2599,7 +2625,7 @@
         <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q7" t="s">
         <v>44</v>
@@ -2613,7 +2639,7 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q8" t="s">
         <v>46</v>
@@ -2627,7 +2653,7 @@
         <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q9" t="s">
         <v>48</v>
@@ -2641,7 +2667,7 @@
         <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q10" t="s">
         <v>50</v>
@@ -2655,7 +2681,7 @@
         <v>61</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q11" t="s">
         <v>62</v>
@@ -2669,7 +2695,7 @@
         <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q12" t="s">
         <v>63</v>
@@ -2683,7 +2709,7 @@
         <v>64</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q13" t="s">
         <v>65</v>
@@ -2697,7 +2723,7 @@
         <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q14" t="s">
         <v>67</v>
@@ -2711,7 +2737,7 @@
         <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q15" t="s">
         <v>69</v>
@@ -2725,7 +2751,7 @@
         <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q16" t="s">
         <v>71</v>
@@ -2739,7 +2765,7 @@
         <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q17" t="s">
         <v>73</v>
@@ -2753,7 +2779,7 @@
         <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q18" t="s">
         <v>76</v>
@@ -2767,7 +2793,7 @@
         <v>77</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q19" t="s">
         <v>78</v>
@@ -2781,7 +2807,7 @@
         <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q20" t="s">
         <v>80</v>
@@ -2795,7 +2821,7 @@
         <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q21" t="s">
         <v>82</v>
@@ -2809,7 +2835,7 @@
         <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q22" t="s">
         <v>84</v>
@@ -2823,7 +2849,7 @@
         <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q23" t="s">
         <v>86</v>
@@ -2837,7 +2863,7 @@
         <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q24" t="s">
         <v>88</v>
@@ -2851,7 +2877,7 @@
         <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q25" t="s">
         <v>90</v>
@@ -2865,7 +2891,7 @@
         <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q26" t="s">
         <v>94</v>
@@ -2879,7 +2905,7 @@
         <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q27" t="s">
         <v>71</v>
@@ -2893,7 +2919,7 @@
         <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q28" t="s">
         <v>73</v>
@@ -2907,13 +2933,13 @@
         <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>410</v>
       </c>
       <c r="Q29" t="s">
         <v>193</v>
@@ -2927,7 +2953,7 @@
         <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
@@ -2947,7 +2973,7 @@
         <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q31" t="s">
         <v>98</v>
@@ -2961,7 +2987,7 @@
         <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q32" t="s">
         <v>100</v>
@@ -2975,7 +3001,7 @@
         <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q33" t="s">
         <v>102</v>
@@ -2989,7 +3015,7 @@
         <v>103</v>
       </c>
       <c r="C34" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q34" t="s">
         <v>104</v>
@@ -3003,7 +3029,7 @@
         <v>105</v>
       </c>
       <c r="C35" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q35" t="s">
         <v>106</v>
@@ -3017,7 +3043,7 @@
         <v>107</v>
       </c>
       <c r="C36" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q36" t="s">
         <v>111</v>
@@ -3031,7 +3057,7 @@
         <v>108</v>
       </c>
       <c r="C37" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q37" t="s">
         <v>71</v>
@@ -3045,7 +3071,7 @@
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q38" t="s">
         <v>110</v>
@@ -3059,7 +3085,7 @@
         <v>112</v>
       </c>
       <c r="C39" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q39" t="s">
         <v>113</v>
@@ -3073,7 +3099,7 @@
         <v>114</v>
       </c>
       <c r="C40" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q40" t="s">
         <v>115</v>
@@ -3087,7 +3113,7 @@
         <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q41" t="s">
         <v>117</v>
@@ -3101,7 +3127,7 @@
         <v>118</v>
       </c>
       <c r="C42" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q42" t="s">
         <v>119</v>
@@ -3115,7 +3141,7 @@
         <v>120</v>
       </c>
       <c r="C43" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q43" t="s">
         <v>123</v>
@@ -3129,7 +3155,7 @@
         <v>121</v>
       </c>
       <c r="C44" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q44" t="s">
         <v>71</v>
@@ -3143,7 +3169,7 @@
         <v>122</v>
       </c>
       <c r="C45" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q45" t="s">
         <v>73</v>
@@ -3157,7 +3183,7 @@
         <v>124</v>
       </c>
       <c r="C46" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q46" t="s">
         <v>128</v>
@@ -3171,7 +3197,7 @@
         <v>125</v>
       </c>
       <c r="C47" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q47" t="s">
         <v>129</v>
@@ -3185,7 +3211,7 @@
         <v>126</v>
       </c>
       <c r="C48" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q48" t="s">
         <v>71</v>
@@ -3199,7 +3225,7 @@
         <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q49" t="s">
         <v>130</v>
@@ -3213,7 +3239,7 @@
         <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q50" t="s">
         <v>143</v>
@@ -3227,7 +3253,7 @@
         <v>132</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q51" t="s">
         <v>71</v>
@@ -3241,7 +3267,7 @@
         <v>133</v>
       </c>
       <c r="C52" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q52" t="s">
         <v>139</v>
@@ -3255,7 +3281,7 @@
         <v>134</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q53" t="s">
         <v>140</v>
@@ -3269,7 +3295,7 @@
         <v>135</v>
       </c>
       <c r="C54" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q54" t="s">
         <v>142</v>
@@ -3283,7 +3309,7 @@
         <v>136</v>
       </c>
       <c r="C55" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q55" t="s">
         <v>110</v>
@@ -3297,7 +3323,7 @@
         <v>137</v>
       </c>
       <c r="C56" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q56" t="s">
         <v>141</v>
@@ -3311,7 +3337,7 @@
         <v>138</v>
       </c>
       <c r="C57" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q57" t="s">
         <v>142</v>
@@ -3325,7 +3351,7 @@
         <v>152</v>
       </c>
       <c r="C58" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q58" t="s">
         <v>154</v>
@@ -3339,7 +3365,7 @@
         <v>153</v>
       </c>
       <c r="C59" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q59" t="s">
         <v>155</v>
@@ -3353,7 +3379,7 @@
         <v>156</v>
       </c>
       <c r="C60" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q60" t="s">
         <v>71</v>
@@ -3367,7 +3393,7 @@
         <v>157</v>
       </c>
       <c r="C61" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q61" t="s">
         <v>130</v>
@@ -3381,7 +3407,7 @@
         <v>144</v>
       </c>
       <c r="C62" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q62" t="s">
         <v>158</v>
@@ -3395,7 +3421,7 @@
         <v>145</v>
       </c>
       <c r="C63" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q63" t="s">
         <v>160</v>
@@ -3409,7 +3435,7 @@
         <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q64" t="s">
         <v>159</v>
@@ -3423,7 +3449,7 @@
         <v>161</v>
       </c>
       <c r="C65" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q65" t="s">
         <v>162</v>
@@ -3437,7 +3463,7 @@
         <v>147</v>
       </c>
       <c r="C66" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q66" t="s">
         <v>71</v>
@@ -3451,7 +3477,7 @@
         <v>148</v>
       </c>
       <c r="C67" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q67" t="s">
         <v>163</v>
@@ -3465,7 +3491,7 @@
         <v>149</v>
       </c>
       <c r="C68" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q68" t="s">
         <v>164</v>
@@ -3479,7 +3505,7 @@
         <v>150</v>
       </c>
       <c r="C69" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q69" t="s">
         <v>165</v>
@@ -3493,7 +3519,7 @@
         <v>166</v>
       </c>
       <c r="C70" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q70" t="s">
         <v>167</v>
@@ -3507,7 +3533,7 @@
         <v>151</v>
       </c>
       <c r="C71" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q71" t="s">
         <v>110</v>
@@ -3521,7 +3547,7 @@
         <v>168</v>
       </c>
       <c r="C72" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q72" t="s">
         <v>169</v>
@@ -3535,7 +3561,7 @@
         <v>170</v>
       </c>
       <c r="C73" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q73" t="s">
         <v>171</v>
@@ -3549,7 +3575,7 @@
         <v>172</v>
       </c>
       <c r="C74" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q74" t="s">
         <v>173</v>
@@ -3563,7 +3589,7 @@
         <v>174</v>
       </c>
       <c r="C75" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q75" t="s">
         <v>175</v>
@@ -3577,7 +3603,7 @@
         <v>176</v>
       </c>
       <c r="C76" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q76" t="s">
         <v>177</v>
@@ -3591,7 +3617,7 @@
         <v>178</v>
       </c>
       <c r="C77" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q77" t="s">
         <v>179</v>
@@ -3605,7 +3631,7 @@
         <v>180</v>
       </c>
       <c r="C78" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q78" t="s">
         <v>181</v>
@@ -3619,7 +3645,7 @@
         <v>182</v>
       </c>
       <c r="C79" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q79" t="s">
         <v>183</v>
@@ -3633,7 +3659,7 @@
         <v>184</v>
       </c>
       <c r="C80" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q80" t="s">
         <v>187</v>
@@ -3647,7 +3673,7 @@
         <v>185</v>
       </c>
       <c r="C81" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q81" t="s">
         <v>71</v>
@@ -3661,7 +3687,7 @@
         <v>186</v>
       </c>
       <c r="C82" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q82" t="s">
         <v>186</v>
@@ -3675,13 +3701,13 @@
         <v>95</v>
       </c>
       <c r="C83" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="D83" t="s">
         <v>41</v>
       </c>
       <c r="E83" t="s">
-        <v>202</v>
+        <v>411</v>
       </c>
       <c r="Q83" t="s">
         <v>192</v>
@@ -3695,7 +3721,7 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q84" t="s">
         <v>191</v>
@@ -3709,7 +3735,7 @@
         <v>19</v>
       </c>
       <c r="C85" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="F85" t="b">
         <v>1</v>
@@ -3729,7 +3755,7 @@
         <v>20</v>
       </c>
       <c r="C86" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q86" t="s">
         <v>195</v>
@@ -3743,7 +3769,7 @@
         <v>196</v>
       </c>
       <c r="C87" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q87" t="s">
         <v>198</v>
@@ -3757,7 +3783,7 @@
         <v>197</v>
       </c>
       <c r="C88" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q88" t="s">
         <v>199</v>
@@ -3771,7 +3797,7 @@
         <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q89" t="s">
         <v>205</v>
@@ -3785,7 +3811,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q90" t="s">
         <v>231</v>
@@ -3799,7 +3825,7 @@
         <v>21</v>
       </c>
       <c r="C91" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q91" t="s">
         <v>232</v>
@@ -3813,7 +3839,7 @@
         <v>200</v>
       </c>
       <c r="C92" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q92" t="s">
         <v>234</v>
@@ -3827,7 +3853,7 @@
         <v>201</v>
       </c>
       <c r="C93" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q93" t="s">
         <v>233</v>
@@ -3841,13 +3867,13 @@
         <v>206</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="D94" t="s">
         <v>41</v>
       </c>
       <c r="E94" t="s">
-        <v>203</v>
+        <v>412</v>
       </c>
       <c r="Q94" t="s">
         <v>235</v>
@@ -3861,7 +3887,7 @@
         <v>207</v>
       </c>
       <c r="C95" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="F95" t="b">
         <v>1</v>
@@ -3881,7 +3907,7 @@
         <v>208</v>
       </c>
       <c r="C96" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q96" t="s">
         <v>236</v>
@@ -3895,7 +3921,7 @@
         <v>209</v>
       </c>
       <c r="C97" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q97" t="s">
         <v>237</v>
@@ -3909,7 +3935,7 @@
         <v>210</v>
       </c>
       <c r="C98" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q98" t="s">
         <v>238</v>
@@ -3923,7 +3949,7 @@
         <v>32</v>
       </c>
       <c r="C99" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q99" t="s">
         <v>239</v>
@@ -3937,7 +3963,7 @@
         <v>34</v>
       </c>
       <c r="C100" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q100" t="s">
         <v>239</v>
@@ -3951,7 +3977,7 @@
         <v>211</v>
       </c>
       <c r="C101" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q101" t="s">
         <v>240</v>
@@ -3965,7 +3991,7 @@
         <v>20</v>
       </c>
       <c r="C102" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q102" t="s">
         <v>241</v>
@@ -3979,7 +4005,7 @@
         <v>196</v>
       </c>
       <c r="C103" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q103" t="s">
         <v>242</v>
@@ -3993,7 +4019,7 @@
         <v>27</v>
       </c>
       <c r="C104" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q104" t="s">
         <v>243</v>
@@ -4007,7 +4033,7 @@
         <v>23</v>
       </c>
       <c r="C105" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q105" t="s">
         <v>244</v>
@@ -4021,7 +4047,7 @@
         <v>22</v>
       </c>
       <c r="C106" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q106" t="s">
         <v>245</v>
@@ -4035,7 +4061,7 @@
         <v>21</v>
       </c>
       <c r="C107" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q107" t="s">
         <v>232</v>
@@ -4049,7 +4075,7 @@
         <v>201</v>
       </c>
       <c r="C108" t="s">
-        <v>204</v>
+        <v>413</v>
       </c>
       <c r="Q108" t="s">
         <v>233</v>
@@ -4063,7 +4089,7 @@
         <v>28</v>
       </c>
       <c r="C109" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="F109" t="b">
         <v>1</v>
@@ -4083,7 +4109,7 @@
         <v>30</v>
       </c>
       <c r="C110" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q110" t="s">
         <v>239</v>
@@ -4097,7 +4123,7 @@
         <v>31</v>
       </c>
       <c r="C111" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q111" t="s">
         <v>247</v>
@@ -4111,7 +4137,7 @@
         <v>33</v>
       </c>
       <c r="C112" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q112" t="s">
         <v>248</v>
@@ -4125,7 +4151,7 @@
         <v>215</v>
       </c>
       <c r="C113" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q113" t="s">
         <v>249</v>
@@ -4139,7 +4165,7 @@
         <v>216</v>
       </c>
       <c r="C114" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q114" t="s">
         <v>250</v>
@@ -4153,7 +4179,7 @@
         <v>217</v>
       </c>
       <c r="C115" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q115" t="s">
         <v>251</v>
@@ -4167,7 +4193,7 @@
         <v>29</v>
       </c>
       <c r="C116" t="s">
-        <v>212</v>
+        <v>414</v>
       </c>
       <c r="Q116" t="s">
         <v>252</v>
@@ -4181,7 +4207,7 @@
         <v>220</v>
       </c>
       <c r="C117" t="s">
-        <v>218</v>
+        <v>415</v>
       </c>
       <c r="F117" t="b">
         <v>1</v>
@@ -4201,7 +4227,7 @@
         <v>221</v>
       </c>
       <c r="C118" t="s">
-        <v>218</v>
+        <v>415</v>
       </c>
       <c r="Q118" t="s">
         <v>253</v>
@@ -4215,7 +4241,7 @@
         <v>222</v>
       </c>
       <c r="C119" t="s">
-        <v>218</v>
+        <v>415</v>
       </c>
       <c r="Q119" t="s">
         <v>253</v>
@@ -4229,7 +4255,7 @@
         <v>30</v>
       </c>
       <c r="C120" t="s">
-        <v>218</v>
+        <v>415</v>
       </c>
       <c r="Q120" t="s">
         <v>239</v>
@@ -4243,7 +4269,7 @@
         <v>223</v>
       </c>
       <c r="C121" t="s">
-        <v>218</v>
+        <v>415</v>
       </c>
       <c r="Q121" t="s">
         <v>254</v>
@@ -4257,7 +4283,7 @@
         <v>24</v>
       </c>
       <c r="C122" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="F122" t="b">
         <v>1</v>
@@ -4277,7 +4303,7 @@
         <v>25</v>
       </c>
       <c r="C123" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="Q123" t="s">
         <v>255</v>
@@ -4291,7 +4317,7 @@
         <v>38</v>
       </c>
       <c r="C124" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="Q124" t="s">
         <v>256</v>
@@ -4305,7 +4331,7 @@
         <v>36</v>
       </c>
       <c r="C125" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="Q125" t="s">
         <v>257</v>
@@ -4319,7 +4345,7 @@
         <v>35</v>
       </c>
       <c r="C126" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="Q126" t="s">
         <v>258</v>
@@ -4333,7 +4359,7 @@
         <v>37</v>
       </c>
       <c r="C127" t="s">
-        <v>224</v>
+        <v>416</v>
       </c>
       <c r="Q127" t="s">
         <v>259</v>
@@ -4347,7 +4373,7 @@
         <v>228</v>
       </c>
       <c r="C128" t="s">
-        <v>226</v>
+        <v>417</v>
       </c>
       <c r="F128" t="b">
         <v>1</v>
@@ -4367,7 +4393,7 @@
         <v>229</v>
       </c>
       <c r="C129" t="s">
-        <v>226</v>
+        <v>417</v>
       </c>
       <c r="Q129" t="s">
         <v>260</v>
@@ -4381,7 +4407,7 @@
         <v>230</v>
       </c>
       <c r="C130" t="s">
-        <v>226</v>
+        <v>417</v>
       </c>
       <c r="Q130" t="s">
         <v>261</v>
@@ -4395,7 +4421,7 @@
         <v>38</v>
       </c>
       <c r="C131" t="s">
-        <v>226</v>
+        <v>417</v>
       </c>
       <c r="Q131" t="s">
         <v>262</v>

</xml_diff>